<commit_message>
Added property to help with stimuli sorting
</commit_message>
<xml_diff>
--- a/stimuli/rmet/mrmet.xlsx
+++ b/stimuli/rmet/mrmet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/callithrix/Documents/Projects/Pontine_7T/code/shared/experiment/mdtb_reduced/stimuli/rmet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/callithrix/code/Python/MultiTaskBattery/stimuli/rmet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B6BD12E-80BA-5D40-B02D-C59CB83896B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438BA18A-C7A3-094D-A3B6-42CED9FD4089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{AFCBA1B3-1B2F-214B-96A6-B2B018C4155E}"/>
+    <workbookView xWindow="-51200" yWindow="-4220" windowWidth="25600" windowHeight="28300" xr2:uid="{AFCBA1B3-1B2F-214B-96A6-B2B018C4155E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195CDD08-62A2-3A47-BEFE-21EC087C6185}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>